<commit_message>
common purchese method in functionallibrary.java and added locators in environmental properties
</commit_message>
<xml_diff>
--- a/TestInput/HybridTest.xlsx
+++ b/TestInput/HybridTest.xlsx
@@ -11,13 +11,14 @@
     <sheet name="ApplicationLogin" sheetId="2" r:id="rId2"/>
     <sheet name="SupplierCreation" sheetId="3" r:id="rId3"/>
     <sheet name="StockCategories" sheetId="4" r:id="rId4"/>
+    <sheet name="Purchases" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="186">
   <si>
     <t>TCID</t>
   </si>
@@ -398,6 +399,183 @@
   </si>
   <si>
     <t>Close browser</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>Object_Type</t>
+  </si>
+  <si>
+    <t>Open Browser</t>
+  </si>
+  <si>
+    <t>Open Application</t>
+  </si>
+  <si>
+    <t>Wait For Username</t>
+  </si>
+  <si>
+    <t>Enter Username</t>
+  </si>
+  <si>
+    <t>Wait For Password</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Entert Password</t>
+  </si>
+  <si>
+    <t>Click On Login</t>
+  </si>
+  <si>
+    <t>Wait For Purchases</t>
+  </si>
+  <si>
+    <t>.//*[@id='mi_a_purchases']/a</t>
+  </si>
+  <si>
+    <t>Click On Purchases</t>
+  </si>
+  <si>
+    <t>Wait For Add Purchases</t>
+  </si>
+  <si>
+    <t>.//*[@id='ewContentColumn']/div[3]/div[1]/div[1]/div[2]/div/a</t>
+  </si>
+  <si>
+    <t>Click On Add Purchases</t>
+  </si>
+  <si>
+    <t>Capture Purchase Number</t>
+  </si>
+  <si>
+    <t>.//*[@id='x_Purchase_Number']</t>
+  </si>
+  <si>
+    <t>wait For Calender</t>
+  </si>
+  <si>
+    <t>.//*[@id='el_a_purchases_Purchase_Date']/div/span/button</t>
+  </si>
+  <si>
+    <t>Click on Calender</t>
+  </si>
+  <si>
+    <t>Select Date</t>
+  </si>
+  <si>
+    <t>calenderhandling</t>
+  </si>
+  <si>
+    <t>html/body/div[17]/table/tbody/tr/td</t>
+  </si>
+  <si>
+    <t>Wait For SupplierId</t>
+  </si>
+  <si>
+    <t>.//*[@id='x_Supplier_ID']</t>
+  </si>
+  <si>
+    <t>Select SupplierId</t>
+  </si>
+  <si>
+    <t>dropDownAction</t>
+  </si>
+  <si>
+    <t>Select Notes</t>
+  </si>
+  <si>
+    <t>.//*[@id='x_Notes']</t>
+  </si>
+  <si>
+    <t>Mobile_Item</t>
+  </si>
+  <si>
+    <t>Supplier Number</t>
+  </si>
+  <si>
+    <t>.//*[@id='x1_Supplier_Number']</t>
+  </si>
+  <si>
+    <t>StockItem</t>
+  </si>
+  <si>
+    <t>.//*[@id='x1_Stock_Item']</t>
+  </si>
+  <si>
+    <t>Purchasing Quantity</t>
+  </si>
+  <si>
+    <t>.//*[@id='x1_Purchasing_Quantity']</t>
+  </si>
+  <si>
+    <t>Supplier Number2</t>
+  </si>
+  <si>
+    <t>.//*[@id='x2_Supplier_Number']</t>
+  </si>
+  <si>
+    <t>StockItem2</t>
+  </si>
+  <si>
+    <t>.//*[@id='x2_Stock_Item']</t>
+  </si>
+  <si>
+    <t>Purchasing Quantity2</t>
+  </si>
+  <si>
+    <t>.//*[@id='x2_Purchasing_Quantity']</t>
+  </si>
+  <si>
+    <t>Wait For Total Payment</t>
+  </si>
+  <si>
+    <t>.//*[@id='x_Total_Payment']</t>
+  </si>
+  <si>
+    <t>Enter Total Payment</t>
+  </si>
+  <si>
+    <t>Delete Record</t>
+  </si>
+  <si>
+    <t>.//*[@id='r3_a_purchases_detail']/td[1]/div/a/span</t>
+  </si>
+  <si>
+    <t>Confirm Delete</t>
+  </si>
+  <si>
+    <t>html/body/div[.]/div[2]/div/div[4]/div[2]/button[1]</t>
+  </si>
+  <si>
+    <t>Click On Add</t>
+  </si>
+  <si>
+    <t>.//*[@id='btnAction']</t>
+  </si>
+  <si>
+    <t>Add New Record</t>
+  </si>
+  <si>
+    <t>html/body/div[19]/div[2]/div/div[4]/div[2]/button[1]</t>
+  </si>
+  <si>
+    <t>Wait For Alert</t>
+  </si>
+  <si>
+    <t>(.//*[text()='OK'])[6]</t>
+  </si>
+  <si>
+    <t>Add Sucessful</t>
+  </si>
+  <si>
+    <t>Click On Logout</t>
+  </si>
+  <si>
+    <t>.//*[@id='mi_logout']/a</t>
   </si>
 </sst>
 </file>
@@ -510,7 +688,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,6 +699,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -816,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,6 +1070,17 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1944,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2377,4 +2572,677 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.5703125" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="11">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="A6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="11">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="A7" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="A9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="A10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="7">
+        <v>10</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75">
+      <c r="A11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75">
+      <c r="A12" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="9">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75">
+      <c r="A13" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="A14" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="A15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="9">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="A16" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75">
+      <c r="A17" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="12">
+        <v>29</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75">
+      <c r="A18" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="9">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75">
+      <c r="A19" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="9">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75">
+      <c r="A21" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75">
+      <c r="A22" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="A23" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75">
+      <c r="A24" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75">
+      <c r="A25" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="9">
+        <v>3</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75">
+      <c r="A26" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="9">
+        <v>3</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75">
+      <c r="A27" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" s="13">
+        <v>2</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75">
+      <c r="A28" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="9">
+        <v>12000</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.75">
+      <c r="A29" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" ht="18.75">
+      <c r="A30" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.75">
+      <c r="A31" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.75">
+      <c r="A32" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" ht="18.75">
+      <c r="A33" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" s="7">
+        <v>10</v>
+      </c>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" ht="18.75">
+      <c r="A34" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" ht="18.75">
+      <c r="A35" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="7">
+        <v>5</v>
+      </c>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" ht="18.75">
+      <c r="A36" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>